<commit_message>
not finished but last day :(
</commit_message>
<xml_diff>
--- a/SQL Excel/easy_sql.xlsx
+++ b/SQL Excel/easy_sql.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanuele.iaccarino\Downloads\Json_Pipeline_associare_tabelle_Source_Destination\SQL Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC881CA-36BA-4E29-90E6-354DDA260C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA69A76-C4C3-419C-ADFC-BA434758F348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,28 +28,28 @@
     <t>target_column</t>
   </si>
   <si>
-    <t>#TMS_CARICAMENTO#.</t>
-  </si>
-  <si>
-    <t>#COD_SIST_ALIMNTNT#.</t>
-  </si>
-  <si>
-    <t>#$BQ_PROJID_T4777A#.#$BQ_DSNAME_T4777A#.VD_T4_DB_PSET.NOM_PSET</t>
-  </si>
-  <si>
-    <t>#$BQ_PROJID_T4777A#.#$BQ_DSNAME_T4777A#.VD_T4_DB_PSET.COD_PSET</t>
-  </si>
-  <si>
-    <t>COD_KEY_PIAZZA_REGOLAMENTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NUM_AA_TT</t>
-  </si>
-  <si>
-    <t>#COD_SIST_ALIMNTNT#</t>
-  </si>
-  <si>
-    <t>#COD_SSA_PROVNNZ#</t>
+    <t>202004142359.</t>
+  </si>
+  <si>
+    <t>TOP.</t>
+  </si>
+  <si>
+    <t>prj-isp-t4777-appl-svil-001.T4777W.VD_T4_DB_PSET.NOM_PSET</t>
+  </si>
+  <si>
+    <t>prj-isp-t4777-appl-svil-001.T4777W.VD_T4_DB_PSET.COD_PSET</t>
+  </si>
+  <si>
+    <t>NUM_AA_TT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> COD_KEY_PIAZZA_REGOLAMENTO</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>T4</t>
   </si>
   <si>
     <t>num_aa_tt</t>
@@ -449,8 +449,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="66.36328125" customWidth="1"/>
-    <col min="2" max="2" width="33.08984375" customWidth="1"/>
+    <col min="1" max="1" width="55.7265625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>